<commit_message>
Add problem statement and SQL scripts for summarizing vehicle repair data by velocity
</commit_message>
<xml_diff>
--- a/Summarize_Levels_Velocity/Problem_Statement.xlsx
+++ b/Summarize_Levels_Velocity/Problem_Statement.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\30DaySQLQueryChallenge - techTFQ\new\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\30DaySQLQueryChallenge - techTFQ\Summarize_Levels_Velocity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA24D7DD-BF73-4874-9C94-283ECD5CAA63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68243F04-4D16-496E-A9FE-C4DDDF2D7A92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{67788DE1-2A4F-384B-B90C-C7BD7F35B3F8}"/>
   </bookViews>
@@ -128,7 +128,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>Video #9</t>
+      <t>#</t>
     </r>
     <r>
       <rPr>
@@ -517,6 +517,78 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -534,78 +606,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -944,7 +944,7 @@
   <dimension ref="B1:L34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:H1"/>
+      <selection activeCell="B2" sqref="B2:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -957,84 +957,84 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.3">
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="2:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
     </row>
     <row r="3" spans="2:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
     </row>
     <row r="4" spans="2:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
     </row>
     <row r="6" spans="2:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="7" spans="2:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="19"/>
-      <c r="I7" s="6" t="s">
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="29"/>
+      <c r="I7" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="8"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="32"/>
     </row>
     <row r="8" spans="2:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="F8" s="10" t="s">
         <v>15</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="20" t="s">
+      <c r="J8" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="20" t="s">
+      <c r="K8" s="11" t="s">
         <v>18</v>
       </c>
       <c r="L8" s="3" t="s">
@@ -1042,286 +1042,286 @@
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="22">
+      <c r="D9" s="13">
         <v>2022</v>
       </c>
-      <c r="E9" s="22" t="s">
+      <c r="E9" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="23" t="s">
+      <c r="F9" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="I9" s="24">
+      <c r="I9" s="15">
         <v>50</v>
       </c>
-      <c r="J9" s="25">
+      <c r="J9" s="16">
         <v>0</v>
       </c>
-      <c r="K9" s="25">
+      <c r="K9" s="16">
         <v>1</v>
       </c>
-      <c r="L9" s="26">
+      <c r="L9" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C10" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="22">
+      <c r="D10" s="13">
         <v>2022</v>
       </c>
-      <c r="E10" s="22" t="s">
+      <c r="E10" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="23">
+      <c r="F10" s="14">
         <v>90</v>
       </c>
-      <c r="I10" s="27">
+      <c r="I10" s="18">
         <v>70</v>
       </c>
-      <c r="J10" s="28">
+      <c r="J10" s="19">
         <v>0</v>
       </c>
-      <c r="K10" s="28">
+      <c r="K10" s="19">
         <v>1</v>
       </c>
-      <c r="L10" s="29">
+      <c r="L10" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="22">
+      <c r="D11" s="13">
         <v>2023</v>
       </c>
-      <c r="E11" s="22" t="s">
+      <c r="E11" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="23" t="s">
+      <c r="F11" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I11" s="27">
+      <c r="I11" s="18">
         <v>80</v>
       </c>
-      <c r="J11" s="28">
+      <c r="J11" s="19">
         <v>1</v>
       </c>
-      <c r="K11" s="28">
+      <c r="K11" s="19">
         <v>0</v>
       </c>
-      <c r="L11" s="29">
+      <c r="L11" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="22">
+      <c r="D12" s="13">
         <v>2023</v>
       </c>
-      <c r="E12" s="22" t="s">
+      <c r="E12" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="23">
+      <c r="F12" s="14">
         <v>80</v>
       </c>
-      <c r="I12" s="30">
+      <c r="I12" s="21">
         <v>90</v>
       </c>
-      <c r="J12" s="31">
+      <c r="J12" s="22">
         <v>2</v>
       </c>
-      <c r="K12" s="31">
+      <c r="K12" s="22">
         <v>0</v>
       </c>
-      <c r="L12" s="32">
+      <c r="L12" s="23">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="22">
+      <c r="D13" s="13">
         <v>2024</v>
       </c>
-      <c r="E13" s="22" t="s">
+      <c r="E13" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F13" s="23" t="s">
+      <c r="F13" s="14" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="C14" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="22">
+      <c r="D14" s="13">
         <v>2024</v>
       </c>
-      <c r="E14" s="22" t="s">
+      <c r="E14" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F14" s="23">
+      <c r="F14" s="14">
         <v>70</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="22" t="s">
+      <c r="C15" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D15" s="22">
+      <c r="D15" s="13">
         <v>2022</v>
       </c>
-      <c r="E15" s="22" t="s">
+      <c r="E15" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F15" s="23" t="s">
+      <c r="F15" s="14" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="C16" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="22">
+      <c r="D16" s="13">
         <v>2022</v>
       </c>
-      <c r="E16" s="22" t="s">
+      <c r="E16" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F16" s="23">
+      <c r="F16" s="14">
         <v>90</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="22">
+      <c r="D17" s="13">
         <v>2023</v>
       </c>
-      <c r="E17" s="22" t="s">
+      <c r="E17" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F17" s="23" t="s">
+      <c r="F17" s="14" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="22" t="s">
+      <c r="C18" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D18" s="22">
+      <c r="D18" s="13">
         <v>2023</v>
       </c>
-      <c r="E18" s="22" t="s">
+      <c r="E18" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F18" s="23">
+      <c r="F18" s="14">
         <v>50</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B19" s="21" t="s">
+      <c r="B19" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="22" t="s">
+      <c r="C19" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D19" s="22">
+      <c r="D19" s="13">
         <v>2024</v>
       </c>
-      <c r="E19" s="22" t="s">
+      <c r="E19" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F19" s="23" t="s">
+      <c r="F19" s="14" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="20" spans="2:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="33" t="s">
+      <c r="B20" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="34" t="s">
+      <c r="C20" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="34">
+      <c r="D20" s="25">
         <v>2024</v>
       </c>
-      <c r="E20" s="34" t="s">
+      <c r="E20" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="F20" s="35">
+      <c r="F20" s="26">
         <v>80</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
     </row>
     <row r="33" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
     </row>
     <row r="34" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1331,5 +1331,6 @@
     <mergeCell ref="B2:H4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>